<commit_message>
Updated FSSAI number, and NULL values
</commit_message>
<xml_diff>
--- a/consolidated_invoice_details.xlsx
+++ b/consolidated_invoice_details.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:V25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,73 +558,299 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20.54</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>102700</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>11521018000014</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>29-07-2023</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (MANKOLI) AVENUE SUPERMARTS LTD. (MANKOLI)
+MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2 MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2
+ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI
+DIST-THANE. 421302 DIST-THANE. 421302</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>79</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>20.54</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>102700</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>570</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>11521018000014</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>25-07-2023</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (MANKOLI) AVENUE SUPERMARTS LTD. (MANKOLI)
+MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2 MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2
+ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI
+DIST-THANE. 421302 DIST-THANE. 421302</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>154</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>0.260</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>40.04</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>4900</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G4" t="n">
         <v>196196</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>TANISHQ AGRO INDUSTRIES</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>378</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>11518060000388</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>11518036001657</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>17-06-2023</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>27AAKPW5971G1Z1</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>27AACCA8432H1ZQ</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>AAKPW5971G</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>NGPS0-3447D</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>07174-220370</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>AVENUE SUPERMART L.T.D. (DATTAWADI) AVENUE SUPERMART L.T.D. (DATTAWADI)
 SURVEY NO. 52, HISSA NO. 1/1, SURVEY NO. 52, HISSA NO. 1/1,
@@ -632,112 +858,112 @@
 WAREHOUSE, NERE GAON, PUNE: 411033 WAREHOUSE, NERE GAON, PUNE: 411033</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>SAIKRUPA LORRY ARRENGERS</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>Maharashtra (27)</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>MH40BL5917</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>46193MH03</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V4" t="inlineStr">
         <is>
           <t>9321315728</t>
         </is>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>RICE</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>10063090</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>462</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>0.260</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>120.12</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>5150</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G5" t="n">
         <v>618618</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>TANISHQ AGRO INDUSTRIES</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>378</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>11518060000388</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>11518036001657</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>17-06-2023</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>27AAKPW5971G1Z1</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>27AACCA8432H1ZQ</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>AAKPW5971G</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>NGPS0-3447D</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>07174-220370</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>AVENUE SUPERMART L.T.D. (DATTAWADI) AVENUE SUPERMART L.T.D. (DATTAWADI)
 SURVEY NO. 52, HISSA NO. 1/1, SURVEY NO. 52, HISSA NO. 1/1,
@@ -745,29 +971,2289 @@
 WAREHOUSE, NERE GAON, PUNE: 411033 WAREHOUSE, NERE GAON, PUNE: 411033</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>SAIKRUPA LORRY ARRENGERS</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S5" t="inlineStr">
         <is>
           <t>Maharashtra (27)</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="T5" t="inlineStr">
         <is>
           <t>MH40BL5917</t>
         </is>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U5" t="inlineStr">
         <is>
           <t>46193MH03</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V5" t="inlineStr">
         <is>
           <t>9321315728</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>270</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>70.20</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>4900</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>343980</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>427</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>26-06-2023</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>NL01AB5489</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>0652MH24</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>9834822411</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>130.00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>5300</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>689000</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>427</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>26-06-2023</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>NL01AB5489</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>0652MH24</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>9834822411</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>20.00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>102000</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>26-06-2023</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>NL01AB5489</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0652MH24</t>
+        </is>
+      </c>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>9834822411</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>165000</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>26-06-2023</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>NL01AB5489</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0652MH24</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>9834822411</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>80.00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>408000</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>11418850000296</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>30-06-2023</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>23AACCA8432H1ZY</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
+LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
+EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
+VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>SINGH TRANSPORT</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh (23)</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>MP09HG9183</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>6913MP09</t>
+        </is>
+      </c>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>9575765937</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>55000</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>443</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>11418850000296</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>30-06-2023</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>23AACCA8432H1ZY</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
+LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
+EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
+VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>SINGH TRANSPORT</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh (23)</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>MP09HG9183</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>6913MP09</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>9575765937</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>5700</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>285000</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>589</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>11521018000014</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>31-07-2023</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (TURBHE) AVENUE SUPERMARTS LTD. (TURBHE)
+C/40 T.T.C. INDUSTRIAL AREA, C/40 T.T.C. INDUSTRIAL AREA,
+PAWNE VILLAGE, TURBHE PAWNE VILLAGE, TURBHE
+NAVI MUMBAI. 400705 NAVI MUMBAI. 400705</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>MH42AQ3092</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>24872MH01</t>
+        </is>
+      </c>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>8930153910</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>175</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>70.00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>5700</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>399000</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>545</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>11514024004727</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>22-07-2023</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD (SHIRDHON) AVENUE SUPERMARTS LTD (SHIRDHON)
+SURVEY NO 14, HISSA NO 5, SHIRDHON, SURVEY NO 14, HISSA NO 5, SHIRDHON,
+TALUKA PANVEL, RAIGAD, TALUKA PANVEL, RAIGAD,
+MAHARASHTRA- 410206 MAHARASHTRA- 410206</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>MH43Y2783</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>68914MH</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>7798169779</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>480</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>124.80</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>5500</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>686400</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>725</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>11521018000014</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>23-08-2023</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (MANKOLI) AVENUE SUPERMARTS LTD. (MANKOLI)
+MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2 MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2
+ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI
+DIST-THANE. 421302 DIST-THANE. 421302</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>5800</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>174000</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>726</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>11516018000577</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>23-08-2023</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD.(VADUNAVGHAR) AVENUE SUPERMARTS LTD.(VADUNAVGHAR)
+BLDG NO. A-8, GALA NO.2 TO 5, SHAKTI BLDG NO. A-8, GALA NO.2 TO 5, SHAKTI
+COMPLEX, SURVEY NO.20 HISA NO.93 COMPLEX, SURVEY NO.20 HISA NO.93
+AT VADUNAVGHAR, BHIVANDI, DIST. THANE AT VADUNAVGHAR, BHIVANDI, DIST. THANE</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>CHANDA BOMBAY ROAD CARRIERS</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>MH04KF9921</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>6679UP72</t>
+        </is>
+      </c>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>9335391304</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>770</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>200.20</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>4900</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>980980</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>727</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>11418850000296</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>23-08-2023</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>23AACCA8432H1ZY</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
+LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
+EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
+VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>SINGH TRANSPORT</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh (23)</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>MH27X6554</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>4655MH</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>8975422171</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>204000</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>728</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>11418850000296</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>23-08-2023</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>23AACCA8432H1ZY</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
+LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
+EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
+VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>SINGH TRANSPORT</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh (23)</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>MH27X6554</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>4655MH</t>
+        </is>
+      </c>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>8975422171</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>5800</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>58000</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>728</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>11418850000296</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>23-08-2023</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>23AACCA8432H1ZY</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (INDORE) AVENUE SUPERMARTS LTD. (INDORE)
+LAND BEARING, SURVEY NO 2, PLOY NO 13, LAND BEARING, SURVEY NO 2, PLOY NO 13,
+EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER, EMPIRE LOGIPARK, AB ROAD, TEHSIL SANWER,
+VILLAGE BARODA ARJUN, DIST- INDORE VILLAGE BARODA ARJUN, DIST- INDORE</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>SINGH TRANSPORT</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Madhya Pradesh (23)</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>MH27X6554</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>4655MH</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>8975422171</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>40.00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>204000</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>732</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>25-08-2023</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>MH26BE7778</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>8943MH26</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>9011262396</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>30.00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>5800</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>174000</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>732</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>11522043000191</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>25-08-2023</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (KOLHAPUR) AVENUE SUPERMARTS LTD. (KOLHAPUR)
+GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR GAT NO.127/2/1 &amp; 127/2/2, SAGLI-KOLHAPUR
+BYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAONBYPASS RD,NR TAMNDALGE GAON, NIMSHIRGAON
+TAL-SHIROL, DIST- KOLHAPUR 416 101. TAL-SHIROL, DIST- KOLHAPUR 416 101.</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>SRI SAI ROADWAYS</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>MH26BE7778</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>8943MH26</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>9011262396</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>50.00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>5800</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>290000</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>733</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>11521018000014</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>25-08-2023</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (MANKOLI) AVENUE SUPERMARTS LTD. (MANKOLI)
+MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2 MAHAVIR COMPLEX GODOWN NO. B1-1 &amp; 2
+ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI ANJUR VILLAGE, MANKOLI NAKA, BHIVANDI
+DIST-THANE. 421302 DIST-THANE. 421302</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>MH04FJ3569</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>45595MH</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>9823507804</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>230</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.260</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>59.80</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>5600</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>334880</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>751</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>11516018000577</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>29-08-2023</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD.(VADUNAVGHAR) AVENUE SUPERMARTS LTD.(VADUNAVGHAR)
+BLDG NO. A-8, GALA NO.2 TO 5, SHAKTI BLDG NO. A-8, GALA NO.2 TO 5, SHAKTI
+COMPLEX, SURVEY NO.20 HISA NO.93 COMPLEX, SURVEY NO.20 HISA NO.93
+AT VADUNAVGHAR, BHIVANDI, DIST. THANE AT VADUNAVGHAR, BHIVANDI, DIST. THANE</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>189</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>75.60</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>5900</t>
+        </is>
+      </c>
+      <c r="G23" t="n">
+        <v>446040</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>760</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>11518016000410</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>31-08-2023</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD. (TURBHE) AVENUE SUPERMARTS LTD. (TURBHE)
+C/40 T.T.C. INDUSTRIAL AREA, C/40 T.T.C. INDUSTRIAL AREA,
+PAWNE VILLAGE, TURBHE PAWNE VILLAGE, TURBHE
+NAVI MUMBAI. 400705 NAVI MUMBAI. 400705</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>MH42AQ3092</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>24872MH</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>8930153910</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>25.20</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>5100</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>128520</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>719</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>11519036001190</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD (AMBI) AVENUE SUPERMARTS LTD (AMBI)
+GUT NO 113, SHED NO 2, MOUZA AMBI, GUT NO 113, SHED NO 2, MOUZA AMBI,
+TALUKA MAVAL, PUNE TALUKA MAVAL, PUNE
+PUNE PMC &amp; RURAL PUNE PMC &amp; RURAL</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>MH43Y5147</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>2371BID</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>9702314642</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>RICE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10063090</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.400</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>15.20</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>5800</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>88160</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>TANISHQ AGRO INDUSTRIES</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>719</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>11519036001190</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>22-08-2023</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>27AAKPW5971G1Z1</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>27AACCA8432H1ZQ</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>AAKPW5971G</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>NGPS0-3447D</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>07174-220370</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>AVENUE SUPERMARTS LTD (AMBI) AVENUE SUPERMARTS LTD (AMBI)
+GUT NO 113, SHED NO 2, MOUZA AMBI, GUT NO 113, SHED NO 2, MOUZA AMBI,
+TALUKA MAVAL, PUNE TALUKA MAVAL, PUNE
+PUNE PMC &amp; RURAL PUNE PMC &amp; RURAL</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>SAIKRUPA LORRY ARRENGERS</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>Maharashtra (27)</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>MH43Y5147</t>
+        </is>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>2371BID</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr">
+        <is>
+          <t>9702314642</t>
         </is>
       </c>
     </row>

</xml_diff>